<commit_message>
Update Test bed to 2.7Vcc
</commit_message>
<xml_diff>
--- a/PCB/PCBv0.1/bq25505 calc.xlsx
+++ b/PCB/PCBv0.1/bq25505 calc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13ba5333fc85f7d9/CiruitProjects/SolarGPS/PCBv1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Veridian-Heliograph\PCB\PCBv0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_EC693EC6EB5D676976AAD33A253F53BD567EA9EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B9EA092-5351-4F1D-B81F-A7A66B38030F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B6763D-6807-4825-B65D-7DF56E606D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="29490" yWindow="4245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bq25505(70" sheetId="1" r:id="rId1"/>
@@ -2234,7 +2234,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O21" sqref="O21"/>
+      <selection pane="topRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2522,7 @@
         <v>44</v>
       </c>
       <c r="O9" s="13">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>1</v>
@@ -2737,15 +2737,15 @@
       </c>
       <c r="O14" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8*$C$1/O9, O8*$C$1/O9-10)</f>
-        <v>5.2433333333333332</v>
+        <v>5.825925925925926</v>
       </c>
       <c r="P14" s="52">
         <f>IF(O14&gt;1,VLOOKUP(O14*10,$AA$26:$AA$132,1)/10,IF(O14&gt;0.099,VLOOKUP(O14*100,$AB$26:$AB$132,1)/100,VLOOKUP(O14*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>5.2299999999999995</v>
+        <v>5.76</v>
       </c>
       <c r="Q14" s="52">
         <f ca="1">IF(O14&gt;1,OFFSET($AA$26,MATCH(O14*10,$AA$26:$AA$132,1),0)/10,IF(O14&gt;0.099, OFFSET($AB$26,MATCH(O14*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O14*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>5.36</v>
+        <v>5.9</v>
       </c>
       <c r="R14" s="54" t="s">
         <v>59</v>
@@ -2885,15 +2885,15 @@
       </c>
       <c r="O16" s="31">
         <f>IF(O8*$C$1/O9&lt;=10, O8-O14, O8-O14-10)</f>
-        <v>7.7566666666666668</v>
+        <v>7.174074074074074</v>
       </c>
       <c r="P16" s="52">
         <f>IF(O16&gt;1,VLOOKUP(O16*10,$AA$26:$AA$132,1)/10,IF(O16&gt;0.099,VLOOKUP(O16*100,$AB$26:$AB$132,1)/100,VLOOKUP(O16*1000,$AB$26:$AB$132,1)/1000))</f>
-        <v>7.68</v>
+        <v>7.15</v>
       </c>
       <c r="Q16" s="52">
         <f ca="1">IF(O16&gt;1,OFFSET($AA$26,MATCH(O16*10,$AA$26:$AA$132,1),0)/10,IF(O16&gt;0.099, OFFSET($AB$26,MATCH(O16*100,$AB$26:$AB$132,1),0)/100,OFFSET($AB$26,MATCH(O16*1000,$AB$26:$AB$132,1),0)/1000))</f>
-        <v>7.87</v>
+        <v>7.32</v>
       </c>
       <c r="R16" s="54" t="s">
         <v>59</v>
@@ -2947,11 +2947,11 @@
       <c r="O17" s="18"/>
       <c r="P17" s="53">
         <f>$C$1*(1+P16/(P14+P15))</f>
-        <v>2.9868260038240919</v>
+        <v>2.711996527777778</v>
       </c>
       <c r="Q17" s="53">
         <f ca="1">$C$1*(1+Q16/(Q14+Q15))</f>
-        <v>2.986623134328358</v>
+        <v>2.7112203389830509</v>
       </c>
       <c r="R17" s="92" t="s">
         <v>1</v>
@@ -3025,7 +3025,7 @@
         <v>45</v>
       </c>
       <c r="O19" s="13">
-        <v>5.23</v>
+        <v>5.76</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>58</v>
@@ -3119,7 +3119,7 @@
         <v>46</v>
       </c>
       <c r="O21" s="13">
-        <v>7.68</v>
+        <v>7.32</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>58</v>
@@ -3211,11 +3211,11 @@
       </c>
       <c r="O23" s="64">
         <f>$C$1*(1+O21/(O19+O20))</f>
-        <v>2.9868260038240915</v>
+        <v>2.7477083333333336</v>
       </c>
       <c r="P23" s="65">
         <f>(O23-O9)/O23*100</f>
-        <v>-0.44107009109474765</v>
+        <v>1.7362953976798892</v>
       </c>
       <c r="Q23" s="94" t="s">
         <v>2</v>
@@ -4274,6 +4274,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Tag xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
+    <Thumbnail xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000F22CD293BA2654895D1449C225927AC" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0bb95fcecff743878fa884d2d9e7463">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6b6f262-197a-43d7-8cc8-2398f9beca90" xmlns:ns3="236af784-b296-4cea-a5d3-eed352c284c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ea284607afbf8a45488423d608757b4" ns2:_="" ns3:_="">
     <xsd:import namespace="e6b6f262-197a-43d7-8cc8-2398f9beca90"/>
@@ -4510,25 +4528,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276C0D19-B21D-4E63-AC38-166F7A170215}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e6b6f262-197a-43d7-8cc8-2398f9beca90"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Tag xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
-    <Thumbnail xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{455C7BEF-6E75-4721-857D-8DB037DB4B67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C222E574-9BC3-4968-98EC-66C15D13800B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4545,22 +4563,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{455C7BEF-6E75-4721-857D-8DB037DB4B67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276C0D19-B21D-4E63-AC38-166F7A170215}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e6b6f262-197a-43d7-8cc8-2398f9beca90"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>